<commit_message>
Validation, make valid and ratios
</commit_message>
<xml_diff>
--- a/examples/data/dataset_basic.xlsx
+++ b/examples/data/dataset_basic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>ec_lab</t>
   </si>
@@ -126,6 +126,21 @@
   </si>
   <si>
     <t>m+ref</t>
+  </si>
+  <si>
+    <t>cl</t>
+  </si>
+  <si>
+    <t>br</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>ph_lab</t>
+  </si>
+  <si>
+    <t>ph_field</t>
   </si>
 </sst>
 </file>
@@ -133,10 +148,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="#.00"/>
-    <numFmt numFmtId="177" formatCode="#."/>
-    <numFmt numFmtId="178" formatCode="m\o\n\th\ d\,\ yyyy"/>
-    <numFmt numFmtId="180" formatCode="_-[$€]* #,##0.00_-;\-[$€]* #,##0.00_-;_-[$€]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#.00"/>
+    <numFmt numFmtId="165" formatCode="#."/>
+    <numFmt numFmtId="166" formatCode="m\o\n\th\ d\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="_-[$€]* #,##0.00_-;\-[$€]* #,##0.00_-;_-[$€]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -468,19 +483,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="180" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -820,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -831,7 +846,7 @@
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -862,8 +877,23 @@
       <c r="J1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -894,8 +924,23 @@
       <c r="J2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -926,8 +971,23 @@
       <c r="J3">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -958,8 +1018,23 @@
       <c r="J4">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>19</v>
+      </c>
+      <c r="L4">
+        <v>224</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>7</v>
+      </c>
+      <c r="O4">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -990,8 +1065,23 @@
       <c r="J5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>31</v>
+      </c>
+      <c r="L5">
+        <v>340</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1022,8 +1112,23 @@
       <c r="J6">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>34</v>
+      </c>
+      <c r="L6">
+        <v>160</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>4.8</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1051,8 +1156,23 @@
       <c r="J7">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <v>41</v>
+      </c>
+      <c r="L7">
+        <v>160</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1080,8 +1200,23 @@
       <c r="J8">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>41</v>
+      </c>
+      <c r="L8">
+        <v>110</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1112,8 +1247,23 @@
       <c r="J9">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>44</v>
+      </c>
+      <c r="L9">
+        <v>150</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1144,8 +1294,23 @@
       <c r="J10">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <v>140</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1176,8 +1341,23 @@
       <c r="J11">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11">
+        <v>45</v>
+      </c>
+      <c r="L11">
+        <v>115</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1208,8 +1388,23 @@
       <c r="J12">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12">
+        <v>33</v>
+      </c>
+      <c r="L12">
+        <v>240</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+      <c r="O12">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1237,8 +1432,23 @@
       <c r="J13">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13">
+        <v>29</v>
+      </c>
+      <c r="L13">
+        <v>200</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1266,8 +1476,23 @@
       <c r="J14">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <v>33</v>
+      </c>
+      <c r="L14">
+        <v>740</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1298,8 +1523,23 @@
       <c r="J15">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>35</v>
+      </c>
+      <c r="L15">
+        <v>1750</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1330,8 +1570,23 @@
       <c r="J16">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>60</v>
+      </c>
+      <c r="L16">
+        <v>10800</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+      <c r="O16">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1362,8 +1617,23 @@
       <c r="J17">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>390</v>
+      </c>
+      <c r="L17">
+        <v>2556</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>8</v>
+      </c>
+      <c r="O17">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1394,8 +1664,23 @@
       <c r="J18">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>1320</v>
+      </c>
+      <c r="L18">
+        <v>212</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>9</v>
+      </c>
+      <c r="O18">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1425,6 +1710,21 @@
       </c>
       <c r="J19">
         <v>390</v>
+      </c>
+      <c r="K19">
+        <v>5285</v>
+      </c>
+      <c r="L19">
+        <v>6845</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19">
+        <v>9.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed xlsx to csv to keep repo small Integrated allowed columns from the files atoms.csv, ions.csv and   other.csv in checking validity of SamplesFrame Updated naming of column headers etc. snake case and only element in   capitals Updated manual indicating this naming convention Added temp to consolidate Implemented calculating of PhreeqPython solution Added tests for PhreeqPython solution
</commit_message>
<xml_diff>
--- a/examples/data/dataset_basic.xlsx
+++ b/examples/data/dataset_basic.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Broncode\HGC\examples\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korevma\Repositories\hgc\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,18 +29,12 @@
     <t>ec_lab</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>ec_field</t>
   </si>
   <si>
     <t>tur</t>
   </si>
   <si>
-    <t>mg</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -128,19 +122,25 @@
     <t>m+ref</t>
   </si>
   <si>
-    <t>cl</t>
-  </si>
-  <si>
-    <t>br</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>ph_lab</t>
   </si>
   <si>
     <t>ph_field</t>
+  </si>
+  <si>
+    <t>temp_lab</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>Na</t>
   </si>
 </sst>
 </file>
@@ -838,7 +838,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -848,101 +848,101 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
-      </c>
       <c r="O1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
       <c r="L2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>105440</v>
@@ -954,7 +954,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>31959</v>
+        <v>33420</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>105330</v>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>105330</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>105330</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>105330</v>
@@ -1174,7 +1174,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>105440</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>105440</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>105440</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>104920</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>107030</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>108050</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>110170</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>112420</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>111740</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>112420</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>112530</v>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>112570</v>

</xml_diff>